<commit_message>
did time betweem releases
</commit_message>
<xml_diff>
--- a/Excel/MonsterHunter_General_Data.xlsx
+++ b/Excel/MonsterHunter_General_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Piercson\Documents\Monster Hunter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Piercson\Desktop\Coding\Python\Monster Hunter\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8828F709-72A0-48B6-8465-D08687BA7105}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7B5DF41-70CA-4702-9AAF-F5698B5C8A8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EB77D3FC-8844-4545-BC75-11F93FD04317}"/>
+    <workbookView xWindow="-16320" yWindow="-4290" windowWidth="16440" windowHeight="28440" xr2:uid="{EB77D3FC-8844-4545-BC75-11F93FD04317}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="37">
   <si>
     <t>Title</t>
   </si>
@@ -142,6 +142,9 @@
   </si>
   <si>
     <t>Monster Hunter Rise</t>
+  </si>
+  <si>
+    <t>Monster Hunter X</t>
   </si>
 </sst>
 </file>
@@ -517,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2BA5D44-CCFB-44EF-8561-F55EB374B85E}">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -936,7 +939,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="B21" t="s">
         <v>7</v>
@@ -976,13 +979,13 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B23" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C23" s="1">
-        <v>42972</v>
+        <v>42566</v>
       </c>
       <c r="D23">
         <v>4</v>
@@ -991,7 +994,7 @@
         <v>14</v>
       </c>
       <c r="F23" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -999,10 +1002,10 @@
         <v>28</v>
       </c>
       <c r="B24" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C24" s="1">
-        <v>43340</v>
+        <v>42972</v>
       </c>
       <c r="D24">
         <v>4</v>
@@ -1016,22 +1019,22 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B25" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C25" s="1">
-        <v>43126</v>
+        <v>43340</v>
       </c>
       <c r="D25">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E25" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="F25" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1039,7 +1042,7 @@
         <v>31</v>
       </c>
       <c r="B26" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C26" s="1">
         <v>43126</v>
@@ -1051,7 +1054,7 @@
         <v>30</v>
       </c>
       <c r="F26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1059,7 +1062,7 @@
         <v>31</v>
       </c>
       <c r="B27" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C27" s="1">
         <v>43126</v>
@@ -1071,7 +1074,7 @@
         <v>30</v>
       </c>
       <c r="F27" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1079,7 +1082,7 @@
         <v>31</v>
       </c>
       <c r="B28" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C28" s="1">
         <v>43126</v>
@@ -1091,18 +1094,18 @@
         <v>30</v>
       </c>
       <c r="F28" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B29" t="s">
-        <v>7</v>
-      </c>
-      <c r="C29" s="3">
-        <v>43714</v>
+        <v>12</v>
+      </c>
+      <c r="C29" s="1">
+        <v>43126</v>
       </c>
       <c r="D29">
         <v>5</v>
@@ -1111,7 +1114,7 @@
         <v>30</v>
       </c>
       <c r="F29" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1119,7 +1122,7 @@
         <v>34</v>
       </c>
       <c r="B30" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C30" s="3">
         <v>43714</v>
@@ -1131,7 +1134,7 @@
         <v>30</v>
       </c>
       <c r="F30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1139,7 +1142,7 @@
         <v>34</v>
       </c>
       <c r="B31" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C31" s="3">
         <v>43714</v>
@@ -1151,7 +1154,7 @@
         <v>30</v>
       </c>
       <c r="F31" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1159,7 +1162,7 @@
         <v>34</v>
       </c>
       <c r="B32" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C32" s="3">
         <v>43714</v>
@@ -1171,27 +1174,27 @@
         <v>30</v>
       </c>
       <c r="F32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B33" t="s">
         <v>12</v>
       </c>
-      <c r="C33" s="1">
-        <v>44281</v>
+      <c r="C33" s="3">
+        <v>43714</v>
       </c>
       <c r="D33">
         <v>5</v>
       </c>
       <c r="E33" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="F33" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1199,7 +1202,7 @@
         <v>35</v>
       </c>
       <c r="B34" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C34" s="1">
         <v>44281</v>
@@ -1211,6 +1214,26 @@
         <v>14</v>
       </c>
       <c r="F34" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" s="1">
+        <v>44281</v>
+      </c>
+      <c r="D35">
+        <v>5</v>
+      </c>
+      <c r="E35" t="s">
+        <v>14</v>
+      </c>
+      <c r="F35" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
f writing monster types
</commit_message>
<xml_diff>
--- a/Excel/MonsterHunter_General_Data.xlsx
+++ b/Excel/MonsterHunter_General_Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Piercson\Desktop\Coding\Python\Monster Hunter\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7B5DF41-70CA-4702-9AAF-F5698B5C8A8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33CEC2B7-6D65-49F5-B4C1-47C2F6BED130}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-16320" yWindow="-4290" windowWidth="16440" windowHeight="28440" xr2:uid="{EB77D3FC-8844-4545-BC75-11F93FD04317}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="40">
   <si>
     <t>Title</t>
   </si>
@@ -145,6 +145,15 @@
   </si>
   <si>
     <t>Monster Hunter X</t>
+  </si>
+  <si>
+    <t>Monster Hunter Portable 2nd</t>
+  </si>
+  <si>
+    <t>Monster Hunter Portable 2nd G</t>
+  </si>
+  <si>
+    <t>Monster Hunter 3 G</t>
   </si>
 </sst>
 </file>
@@ -520,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2BA5D44-CCFB-44EF-8561-F55EB374B85E}">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1237,6 +1246,66 @@
         <v>29</v>
       </c>
     </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36" s="1">
+        <v>39135</v>
+      </c>
+      <c r="D36">
+        <v>2</v>
+      </c>
+      <c r="E36" t="s">
+        <v>14</v>
+      </c>
+      <c r="F36" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37" t="s">
+        <v>7</v>
+      </c>
+      <c r="C37" s="1">
+        <v>39534</v>
+      </c>
+      <c r="D37">
+        <v>2</v>
+      </c>
+      <c r="E37" t="s">
+        <v>14</v>
+      </c>
+      <c r="F37" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>39</v>
+      </c>
+      <c r="B38" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38" s="1">
+        <v>40887</v>
+      </c>
+      <c r="D38">
+        <v>3</v>
+      </c>
+      <c r="E38" t="s">
+        <v>8</v>
+      </c>
+      <c r="F38" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>